<commit_message>
Updates as per Steve Gaul
updates to sheets as provided by steve gaul
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00001.xlsx
+++ b/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00001.xlsx
@@ -268,7 +268,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -537,9 +537,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -574,7 +571,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,19 +1131,19 @@
       <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="32">
         <v>41918</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="33">
         <v>0.94791666666666663</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="32">
         <v>41979</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="23" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="17">
@@ -1153,11 +1153,11 @@
         <v>39</v>
       </c>
       <c r="K2" s="16"/>
-      <c r="L2" s="32">
+      <c r="L2" s="31">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
         <v>44.370366666666669</v>
       </c>
-      <c r="M2" s="32">
+      <c r="M2" s="31">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-124.95005</v>
       </c>
@@ -1211,391 +1211,391 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>311</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>1</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="26">
         <v>50145</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>311</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>1</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>2760</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>117</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>311</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>2760</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>700</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>311</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>2760</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>1.08</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>311</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>1</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>2760</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>3.9E-2</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>311</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>1</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>642931</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>0.61</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>311</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>1</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="26">
         <v>642931</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <v>0.61</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>311</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>1</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>642931</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="28">
         <v>0.61</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>311</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <v>1</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="26">
         <v>642931</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="28">
         <v>0.61</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
     </row>
     <row r="14" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>311</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <v>1</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="26">
         <v>26</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>311</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="21">
         <v>1</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="26">
         <v>9014</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="21">
         <v>311</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>1</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="26">
         <v>311</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update sort.py to overwrite files. Update calibration sheets for various platforms as per Redmine #8310.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00001.xlsx
+++ b/CE05MOAS-GL311/Omaha_Cal_Info_CE05MOAS-GL311_00001.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12708" yWindow="-12" windowWidth="12516" windowHeight="12396" tabRatio="377" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -31,7 +36,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$76</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$230</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -236,9 +241,6 @@
     <t>Oceanus</t>
   </si>
   <si>
-    <t>Anhcor Launch Date</t>
-  </si>
-  <si>
     <t>Anchor Launch Time</t>
   </si>
   <si>
@@ -261,6 +263,9 @@
   </si>
   <si>
     <t>Mooring Serial Number</t>
+  </si>
+  <si>
+    <t>Anchor Launch Date</t>
   </si>
 </sst>
 </file>
@@ -379,7 +384,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,12 +406,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,7 +497,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -521,7 +520,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -556,12 +555,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -574,7 +567,10 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,6 +653,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -704,7 +703,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -739,7 +738,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1068,7 +1067,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,10 +1096,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -1131,13 +1130,13 @@
       <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="30">
         <v>41918</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <v>0.94791666666666663</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="30">
         <v>41979</v>
       </c>
       <c r="G2" s="23" t="s">
@@ -1153,11 +1152,11 @@
         <v>39</v>
       </c>
       <c r="K2" s="16"/>
-      <c r="L2" s="31">
+      <c r="L2" s="29">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
         <v>44.370366666666669</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="29">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-124.95005</v>
       </c>
@@ -1173,7 +1172,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
@@ -1212,7 +1211,7 @@
     </row>
     <row r="2" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="21">
         <v>311</v>
@@ -1246,7 +1245,7 @@
     </row>
     <row r="4" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="21">
         <v>311</v>
@@ -1260,7 +1259,7 @@
       <c r="E4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="28">
         <v>117</v>
       </c>
       <c r="G4" s="19"/>
@@ -1271,7 +1270,7 @@
     </row>
     <row r="5" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="21">
         <v>311</v>
@@ -1285,7 +1284,7 @@
       <c r="E5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="28">
         <v>700</v>
       </c>
       <c r="G5" s="19"/>
@@ -1296,7 +1295,7 @@
     </row>
     <row r="6" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="21">
         <v>311</v>
@@ -1310,7 +1309,7 @@
       <c r="E6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="28">
         <v>1.08</v>
       </c>
       <c r="G6" s="19"/>
@@ -1321,7 +1320,7 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="21">
         <v>311</v>
@@ -1335,7 +1334,7 @@
       <c r="E7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="28">
         <v>3.9E-2</v>
       </c>
       <c r="G7" s="19"/>
@@ -1350,7 +1349,7 @@
       <c r="C8" s="21"/>
       <c r="D8" s="26"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
@@ -1359,7 +1358,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="21">
         <v>311</v>
@@ -1373,7 +1372,7 @@
       <c r="E9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="31">
         <v>0.61</v>
       </c>
       <c r="G9" s="25"/>
@@ -1389,7 +1388,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="21">
         <v>311</v>
@@ -1403,7 +1402,7 @@
       <c r="E10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="31">
         <v>0.61</v>
       </c>
       <c r="G10" s="25"/>
@@ -1419,7 +1418,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="21">
         <v>311</v>
@@ -1433,7 +1432,7 @@
       <c r="E11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="31">
         <v>0.61</v>
       </c>
       <c r="G11" s="25"/>
@@ -1449,7 +1448,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="21">
         <v>311</v>
@@ -1463,7 +1462,7 @@
       <c r="E12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="31">
         <v>0.61</v>
       </c>
       <c r="G12" s="25"/>
@@ -1483,7 +1482,7 @@
       <c r="C13" s="21"/>
       <c r="D13" s="26"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="29"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -1497,7 +1496,7 @@
     </row>
     <row r="14" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="21">
         <v>311</v>
@@ -1531,7 +1530,7 @@
     </row>
     <row r="16" spans="1:16" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="21">
         <v>311</v>
@@ -1565,7 +1564,7 @@
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="21">
         <v>311</v>

</xml_diff>